<commit_message>
configured volunteer view-edit feature
</commit_message>
<xml_diff>
--- a/testData.xlsx
+++ b/testData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kunsa\Desktop\laravel\smitnss\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC756ABC-E76E-449C-BA77-E143C4558E77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B939DD37-033F-4343-8AE7-725FF3F32A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{94DC1226-721B-4661-967B-2B0E57E0D103}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{94DC1226-721B-4661-967B-2B0E57E0D103}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Users" sheetId="1" r:id="rId1"/>
+    <sheet name="Courses" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
   <si>
     <t>Name</t>
   </si>
@@ -114,6 +115,60 @@
   </si>
   <si>
     <t>2022-28</t>
+  </si>
+  <si>
+    <t>COURSE NAME</t>
+  </si>
+  <si>
+    <t>CID</t>
+  </si>
+  <si>
+    <t>MCA</t>
+  </si>
+  <si>
+    <t>MBA</t>
+  </si>
+  <si>
+    <t>BBA</t>
+  </si>
+  <si>
+    <t>MSc Chemistry</t>
+  </si>
+  <si>
+    <t>BSc Chemistry</t>
+  </si>
+  <si>
+    <t>MSc Mathematics</t>
+  </si>
+  <si>
+    <t>BSc Mathematics</t>
+  </si>
+  <si>
+    <t>BSc Physics</t>
+  </si>
+  <si>
+    <t>MSc Physics</t>
+  </si>
+  <si>
+    <t>BTech CSE</t>
+  </si>
+  <si>
+    <t>BTech CE</t>
+  </si>
+  <si>
+    <t>BTech ME</t>
+  </si>
+  <si>
+    <t>BTech AI&amp;DS</t>
+  </si>
+  <si>
+    <t>BTech IT</t>
+  </si>
+  <si>
+    <t>BTech EEE</t>
+  </si>
+  <si>
+    <t>BTech ECE</t>
   </si>
 </sst>
 </file>
@@ -164,13 +219,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -489,7 +547,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A9DF2B9-B565-4A47-8D92-DC6304F87596}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
@@ -691,4 +749,167 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D80A30C2-9AFF-4A20-BE8B-B941F6926369}">
+  <dimension ref="A1:B18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.42578125" style="3" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="3">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>